<commit_message>
updates till config standardisation
</commit_message>
<xml_diff>
--- a/testData/muleguard-reports/CONSOLIDATED-REPORT.xlsx
+++ b/testData/muleguard-reports/CONSOLIDATED-REPORT.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>API Name</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>.\testData\muleguard-reports\customerOrder_V3\report.html</t>
+  </si>
+  <si>
+    <t>edgetest_config</t>
+  </si>
+  <si>
+    <t>.\testData\muleguard-reports\edgetest_config\report.html</t>
   </si>
   <si>
     <t>muleapp1</t>
@@ -182,7 +188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -261,10 +267,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="n" s="3">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="C4" t="n" s="3">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D4" t="n" s="3">
         <v>5.0</v>
@@ -301,13 +307,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="n" s="3">
-        <v>15.0</v>
+        <v>11.0</v>
       </c>
       <c r="C6" t="n" s="3">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="D6" t="n" s="3">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c r="E6" t="s" s="3">
         <v>7</v>
@@ -321,13 +327,13 @@
         <v>17</v>
       </c>
       <c r="B7" t="n" s="3">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
       <c r="C7" t="n" s="3">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7" t="n" s="3">
-        <v>7.0</v>
+        <v>13.0</v>
       </c>
       <c r="E7" t="s" s="3">
         <v>7</v>
@@ -341,13 +347,13 @@
         <v>19</v>
       </c>
       <c r="B8" t="n" s="3">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="C8" t="n" s="3">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D8" t="n" s="3">
-        <v>5.0</v>
+        <v>11.0</v>
       </c>
       <c r="E8" t="s" s="3">
         <v>7</v>
@@ -361,13 +367,13 @@
         <v>21</v>
       </c>
       <c r="B9" t="n" s="3">
-        <v>15.0</v>
+        <v>11.0</v>
       </c>
       <c r="C9" t="n" s="3">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D9" t="n" s="3">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="E9" t="s" s="3">
         <v>7</v>
@@ -381,13 +387,13 @@
         <v>23</v>
       </c>
       <c r="B10" t="n" s="3">
-        <v>7.0</v>
+        <v>15.0</v>
       </c>
       <c r="C10" t="n" s="3">
         <v>2.0</v>
       </c>
       <c r="D10" t="n" s="3">
-        <v>5.0</v>
+        <v>13.0</v>
       </c>
       <c r="E10" t="s" s="3">
         <v>7</v>
@@ -397,20 +403,40 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="4">
+      <c r="A11" t="s" s="3">
         <v>25</v>
       </c>
-      <c r="B11" t="n" s="0">
-        <v>103.0</v>
-      </c>
-      <c r="C11" t="n" s="0">
-        <v>49.0</v>
-      </c>
-      <c r="D11" t="n" s="0">
-        <v>54.0</v>
-      </c>
-      <c r="E11" t="s" s="0">
+      <c r="B11" t="n" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="C11" t="n" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="D11" t="n" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="E11" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s" s="3">
         <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>130.0</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>71.0</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>59.0</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>